<commit_message>
Clean up Physical and Digital Album Sales Files
</commit_message>
<xml_diff>
--- a/Physical Sales 1-1-2021 - 12-31-2022 example.xlsx
+++ b/Physical Sales 1-1-2021 - 12-31-2022 example.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="940" yWindow="1660" windowWidth="28780" windowHeight="23920"/>
+    <workbookView xWindow="2160" yWindow="1780" windowWidth="28780" windowHeight="23920"/>
   </bookViews>
   <sheets>
     <sheet name="RS Physical Sales Template" sheetId="1" r:id="rId1"/>
@@ -45,21 +45,6 @@
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">2-letter alphabetic ISO code (ISO 3166-1-alpha-2 code) for the sales territory
-*Required field
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -113,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -166,7 +151,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -299,7 +284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -313,7 +298,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -327,7 +312,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -370,7 +355,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -393,7 +378,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -432,7 +417,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="669">
   <si>
     <t>artist-name</t>
   </si>
@@ -1914,9 +1899,6 @@
   </si>
   <si>
     <t>net-units</t>
-  </si>
-  <si>
-    <t>country-code</t>
   </si>
   <si>
     <t>product-type</t>
@@ -1926,10 +1908,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>US</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>KERMIT RUFFINS</t>
   </si>
   <si>
@@ -1989,9 +1967,6 @@
   </si>
   <si>
     <t>LP</t>
-  </si>
-  <si>
-    <t>US</t>
   </si>
   <si>
     <t>IRVIN MAYFIELD ORLEANS JAZZ ORCHESTRA</t>
@@ -2501,13 +2476,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -2523,6 +2491,11 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2584,12 +2557,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2897,2493 +2870,2261 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.83203125" customWidth="1"/>
-    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.83203125" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" customWidth="1"/>
+    <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>481</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>485</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
         <v>495</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B2">
+        <v>2022</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>514</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>524</v>
+      </c>
+      <c r="G2" s="7">
+        <v>652905010112</v>
+      </c>
+      <c r="H2" t="s">
+        <v>600</v>
+      </c>
+      <c r="I2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>495</v>
+      </c>
+      <c r="B3">
+        <v>2022</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>512</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>525</v>
+      </c>
+      <c r="G3" s="7">
+        <v>652905010129</v>
+      </c>
+      <c r="H3" t="s">
+        <v>600</v>
+      </c>
+      <c r="I3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>495</v>
+      </c>
+      <c r="B4">
+        <v>2022</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>512</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>526</v>
+      </c>
+      <c r="G4" s="8">
+        <v>652905010228</v>
+      </c>
+      <c r="H4" t="s">
+        <v>601</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>495</v>
+      </c>
+      <c r="B5">
+        <v>2022</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>512</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>527</v>
+      </c>
+      <c r="G5" s="8">
+        <v>652905010327</v>
+      </c>
+      <c r="H5" t="s">
+        <v>602</v>
+      </c>
+      <c r="I5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>495</v>
+      </c>
+      <c r="B6">
+        <v>2022</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>512</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>528</v>
+      </c>
+      <c r="G6" s="8">
+        <v>652905010426</v>
+      </c>
+      <c r="H6" t="s">
+        <v>603</v>
+      </c>
+      <c r="I6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>495</v>
+      </c>
+      <c r="B7">
+        <v>2022</v>
+      </c>
+      <c r="C7">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>514</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>497</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>529</v>
+      </c>
+      <c r="G7" s="8">
+        <v>652905010518</v>
+      </c>
+      <c r="H7" t="s">
+        <v>604</v>
+      </c>
+      <c r="I7">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>495</v>
+      </c>
+      <c r="B8">
+        <v>2022</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>512</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>497</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>530</v>
+      </c>
+      <c r="G8" s="8">
+        <v>652905010525</v>
+      </c>
+      <c r="H8" t="s">
+        <v>604</v>
+      </c>
+      <c r="I8">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>495</v>
+      </c>
+      <c r="B9">
+        <v>2022</v>
+      </c>
+      <c r="C9">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>512</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>531</v>
+      </c>
+      <c r="G9" s="8">
+        <v>652905010624</v>
+      </c>
+      <c r="H9" t="s">
+        <v>605</v>
+      </c>
+      <c r="I9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>495</v>
+      </c>
+      <c r="B10">
+        <v>2022</v>
+      </c>
+      <c r="C10">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>512</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>532</v>
+      </c>
+      <c r="G10" s="8">
+        <v>652905010723</v>
+      </c>
+      <c r="H10" t="s">
+        <v>606</v>
+      </c>
+      <c r="I10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>495</v>
+      </c>
+      <c r="B11">
+        <v>2022</v>
+      </c>
+      <c r="C11">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>512</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>533</v>
+      </c>
+      <c r="G11" s="8">
+        <v>652905010822</v>
+      </c>
+      <c r="H11" t="s">
+        <v>607</v>
+      </c>
+      <c r="I11">
         <v>0</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>495</v>
+      </c>
+      <c r="B12">
+        <v>2022</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>512</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>496</v>
       </c>
-      <c r="B2" t="s">
-        <v>497</v>
-      </c>
-      <c r="C2">
+      <c r="F12" s="12" t="s">
+        <v>534</v>
+      </c>
+      <c r="G12" s="8">
+        <v>652905010914</v>
+      </c>
+      <c r="H12" t="s">
+        <v>608</v>
+      </c>
+      <c r="I12">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>495</v>
+      </c>
+      <c r="B13">
         <v>2022</v>
       </c>
-      <c r="D2">
+      <c r="C13">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D13" t="s">
+        <v>512</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>535</v>
+      </c>
+      <c r="G13" s="8">
+        <v>652905010921</v>
+      </c>
+      <c r="H13" t="s">
+        <v>608</v>
+      </c>
+      <c r="I13">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>495</v>
+      </c>
+      <c r="B14">
+        <v>2022</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>512</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>536</v>
+      </c>
+      <c r="G14" s="8">
+        <v>652905011126</v>
+      </c>
+      <c r="H14" t="s">
+        <v>609</v>
+      </c>
+      <c r="I14">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>495</v>
+      </c>
+      <c r="B15">
+        <v>2022</v>
+      </c>
+      <c r="C15">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>512</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>537</v>
+      </c>
+      <c r="G15" s="8">
+        <v>652905011225</v>
+      </c>
+      <c r="H15" t="s">
+        <v>610</v>
+      </c>
+      <c r="I15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>495</v>
+      </c>
+      <c r="B16">
+        <v>2022</v>
+      </c>
+      <c r="C16">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>512</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>538</v>
+      </c>
+      <c r="G16" s="8">
+        <v>652905011324</v>
+      </c>
+      <c r="H16" t="s">
+        <v>611</v>
+      </c>
+      <c r="I16">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>495</v>
+      </c>
+      <c r="B17">
+        <v>2022</v>
+      </c>
+      <c r="C17">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>512</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>539</v>
+      </c>
+      <c r="G17" s="8">
+        <v>652905011423</v>
+      </c>
+      <c r="H17" t="s">
+        <v>612</v>
+      </c>
+      <c r="I17">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>495</v>
+      </c>
+      <c r="B18">
+        <v>2022</v>
+      </c>
+      <c r="C18">
+        <v>12</v>
+      </c>
+      <c r="D18" t="s">
+        <v>512</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>540</v>
+      </c>
+      <c r="G18" s="8">
+        <v>652905011522</v>
+      </c>
+      <c r="H18" t="s">
+        <v>613</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>495</v>
+      </c>
+      <c r="B19">
+        <v>2022</v>
+      </c>
+      <c r="C19">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
+        <v>512</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>541</v>
+      </c>
+      <c r="G19" s="8">
+        <v>652905020128</v>
+      </c>
+      <c r="H19" t="s">
+        <v>614</v>
+      </c>
+      <c r="I19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>495</v>
+      </c>
+      <c r="B20">
+        <v>2022</v>
+      </c>
+      <c r="C20">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>512</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>498</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>542</v>
+      </c>
+      <c r="G20" s="8">
+        <v>652905020227</v>
+      </c>
+      <c r="H20" t="s">
+        <v>615</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>495</v>
+      </c>
+      <c r="B21">
+        <v>2022</v>
+      </c>
+      <c r="C21">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>512</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>543</v>
+      </c>
+      <c r="G21" s="8">
+        <v>652905020326</v>
+      </c>
+      <c r="H21" t="s">
+        <v>616</v>
+      </c>
+      <c r="I21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>495</v>
+      </c>
+      <c r="B22">
+        <v>2022</v>
+      </c>
+      <c r="C22">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>512</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>544</v>
+      </c>
+      <c r="G22" s="8">
+        <v>652905020425</v>
+      </c>
+      <c r="H22" t="s">
+        <v>617</v>
+      </c>
+      <c r="I22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>495</v>
+      </c>
+      <c r="B23">
+        <v>2022</v>
+      </c>
+      <c r="C23">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
+        <v>512</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>545</v>
+      </c>
+      <c r="G23" s="8">
+        <v>652905020623</v>
+      </c>
+      <c r="H23" t="s">
+        <v>618</v>
+      </c>
+      <c r="I23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>495</v>
+      </c>
+      <c r="B24">
+        <v>2022</v>
+      </c>
+      <c r="C24">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s">
+        <v>512</v>
+      </c>
+      <c r="E24" t="s">
+        <v>499</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>546</v>
+      </c>
+      <c r="G24" s="8">
+        <v>652905030127</v>
+      </c>
+      <c r="H24" t="s">
+        <v>619</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>495</v>
+      </c>
+      <c r="B25">
+        <v>2022</v>
+      </c>
+      <c r="C25">
+        <v>12</v>
+      </c>
+      <c r="D25" t="s">
+        <v>512</v>
+      </c>
+      <c r="E25" t="s">
+        <v>499</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>547</v>
+      </c>
+      <c r="G25" s="8">
+        <v>652905030226</v>
+      </c>
+      <c r="H25" t="s">
+        <v>620</v>
+      </c>
+      <c r="I25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>495</v>
+      </c>
+      <c r="B26">
+        <v>2022</v>
+      </c>
+      <c r="C26">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s">
+        <v>512</v>
+      </c>
+      <c r="E26" t="s">
+        <v>500</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>548</v>
+      </c>
+      <c r="G26" s="8">
+        <v>652905030325</v>
+      </c>
+      <c r="H26" t="s">
+        <v>621</v>
+      </c>
+      <c r="I26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>495</v>
+      </c>
+      <c r="B27">
+        <v>2022</v>
+      </c>
+      <c r="C27">
+        <v>12</v>
+      </c>
+      <c r="D27" t="s">
+        <v>512</v>
+      </c>
+      <c r="E27" t="s">
+        <v>500</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>549</v>
+      </c>
+      <c r="G27" s="8">
+        <v>652905030424</v>
+      </c>
+      <c r="H27" t="s">
+        <v>622</v>
+      </c>
+      <c r="I27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>495</v>
+      </c>
+      <c r="B28">
+        <v>2022</v>
+      </c>
+      <c r="C28">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
+        <v>512</v>
+      </c>
+      <c r="E28" t="s">
+        <v>519</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>550</v>
+      </c>
+      <c r="G28" s="8">
+        <v>652905030523</v>
+      </c>
+      <c r="H28" t="s">
+        <v>623</v>
+      </c>
+      <c r="I28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>495</v>
+      </c>
+      <c r="B29">
+        <v>2022</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
+      </c>
+      <c r="D29" t="s">
+        <v>512</v>
+      </c>
+      <c r="E29" t="s">
+        <v>522</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>551</v>
+      </c>
+      <c r="G29" s="8">
+        <v>652905030622</v>
+      </c>
+      <c r="H29" t="s">
+        <v>624</v>
+      </c>
+      <c r="I29">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>495</v>
+      </c>
+      <c r="B30">
+        <v>2022</v>
+      </c>
+      <c r="C30">
+        <v>12</v>
+      </c>
+      <c r="D30" t="s">
+        <v>512</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>552</v>
+      </c>
+      <c r="G30" s="8">
+        <v>652905040126</v>
+      </c>
+      <c r="H30" t="s">
+        <v>625</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>495</v>
+      </c>
+      <c r="B31">
+        <v>2022</v>
+      </c>
+      <c r="C31">
+        <v>12</v>
+      </c>
+      <c r="D31" t="s">
+        <v>512</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>553</v>
+      </c>
+      <c r="G31" s="8">
+        <v>652905040225</v>
+      </c>
+      <c r="H31" t="s">
+        <v>626</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>495</v>
+      </c>
+      <c r="B32">
+        <v>2022</v>
+      </c>
+      <c r="C32">
+        <v>12</v>
+      </c>
+      <c r="D32" t="s">
+        <v>512</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>554</v>
+      </c>
+      <c r="G32" s="8">
+        <v>652905040324</v>
+      </c>
+      <c r="H32" t="s">
+        <v>627</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>495</v>
+      </c>
+      <c r="B33">
+        <v>2022</v>
+      </c>
+      <c r="C33">
+        <v>12</v>
+      </c>
+      <c r="D33" t="s">
+        <v>512</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>555</v>
+      </c>
+      <c r="G33" s="8">
+        <v>652905040423</v>
+      </c>
+      <c r="H33" t="s">
+        <v>628</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>495</v>
+      </c>
+      <c r="B34">
+        <v>2022</v>
+      </c>
+      <c r="C34">
+        <v>12</v>
+      </c>
+      <c r="D34" t="s">
+        <v>512</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>556</v>
+      </c>
+      <c r="G34" s="8">
+        <v>652905040522</v>
+      </c>
+      <c r="H34" t="s">
+        <v>629</v>
+      </c>
+      <c r="I34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>495</v>
+      </c>
+      <c r="B35">
+        <v>2022</v>
+      </c>
+      <c r="C35">
+        <v>12</v>
+      </c>
+      <c r="D35" t="s">
+        <v>512</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>557</v>
+      </c>
+      <c r="G35" s="10">
+        <v>652905040621</v>
+      </c>
+      <c r="H35" t="s">
+        <v>630</v>
+      </c>
+      <c r="I35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>495</v>
+      </c>
+      <c r="B36">
+        <v>2022</v>
+      </c>
+      <c r="C36">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s">
+        <v>512</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>558</v>
+      </c>
+      <c r="G36" s="10">
+        <v>652905040720</v>
+      </c>
+      <c r="H36" t="s">
+        <v>631</v>
+      </c>
+      <c r="I36">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>495</v>
+      </c>
+      <c r="B37">
+        <v>2022</v>
+      </c>
+      <c r="C37">
+        <v>12</v>
+      </c>
+      <c r="D37" t="s">
+        <v>512</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>559</v>
+      </c>
+      <c r="G37" s="10">
+        <v>652905040836</v>
+      </c>
+      <c r="H37" t="s">
+        <v>632</v>
+      </c>
+      <c r="I37">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>495</v>
+      </c>
+      <c r="B38">
+        <v>2022</v>
+      </c>
+      <c r="C38">
+        <v>12</v>
+      </c>
+      <c r="D38" t="s">
+        <v>512</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>515</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>560</v>
+      </c>
+      <c r="G38" s="10">
+        <v>652905040928</v>
+      </c>
+      <c r="H38" t="s">
+        <v>633</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>495</v>
+      </c>
+      <c r="B39">
+        <v>2022</v>
+      </c>
+      <c r="C39">
+        <v>12</v>
+      </c>
+      <c r="D39" t="s">
+        <v>512</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>561</v>
+      </c>
+      <c r="G39" s="8">
+        <v>652905050125</v>
+      </c>
+      <c r="H39" t="s">
+        <v>634</v>
+      </c>
+      <c r="I39">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
+        <v>495</v>
+      </c>
+      <c r="B40">
+        <v>2022</v>
+      </c>
+      <c r="C40">
+        <v>12</v>
+      </c>
+      <c r="D40" t="s">
+        <v>512</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>562</v>
+      </c>
+      <c r="G40" s="8">
+        <v>652905050224</v>
+      </c>
+      <c r="H40" t="s">
+        <v>635</v>
+      </c>
+      <c r="I40">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>495</v>
+      </c>
+      <c r="B41">
+        <v>2022</v>
+      </c>
+      <c r="C41">
+        <v>12</v>
+      </c>
+      <c r="D41" t="s">
+        <v>512</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>563</v>
+      </c>
+      <c r="G41" s="8">
+        <v>652905050323</v>
+      </c>
+      <c r="H41" t="s">
+        <v>636</v>
+      </c>
+      <c r="I41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
+        <v>495</v>
+      </c>
+      <c r="B42">
+        <v>2022</v>
+      </c>
+      <c r="C42">
+        <v>12</v>
+      </c>
+      <c r="D42" t="s">
+        <v>512</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>564</v>
+      </c>
+      <c r="G42" s="8">
+        <v>652905050422</v>
+      </c>
+      <c r="H42" t="s">
+        <v>637</v>
+      </c>
+      <c r="I42">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
+        <v>495</v>
+      </c>
+      <c r="B43">
+        <v>2022</v>
+      </c>
+      <c r="C43">
+        <v>12</v>
+      </c>
+      <c r="D43" t="s">
+        <v>512</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>565</v>
+      </c>
+      <c r="G43" s="10">
+        <v>652905050521</v>
+      </c>
+      <c r="H43" t="s">
+        <v>638</v>
+      </c>
+      <c r="I43">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>495</v>
+      </c>
+      <c r="B44">
+        <v>2022</v>
+      </c>
+      <c r="C44">
+        <v>12</v>
+      </c>
+      <c r="D44" t="s">
+        <v>512</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>566</v>
+      </c>
+      <c r="G44" s="10">
+        <v>652905050620</v>
+      </c>
+      <c r="H44" t="s">
+        <v>639</v>
+      </c>
+      <c r="I44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>495</v>
+      </c>
+      <c r="B45">
+        <v>2022</v>
+      </c>
+      <c r="C45">
+        <v>12</v>
+      </c>
+      <c r="D45" t="s">
+        <v>512</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>567</v>
+      </c>
+      <c r="G45" s="10">
+        <v>652905050729</v>
+      </c>
+      <c r="H45" t="s">
+        <v>640</v>
+      </c>
+      <c r="I45">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
+        <v>495</v>
+      </c>
+      <c r="B46">
+        <v>2022</v>
+      </c>
+      <c r="C46">
+        <v>12</v>
+      </c>
+      <c r="D46" t="s">
+        <v>512</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>568</v>
+      </c>
+      <c r="G46" s="10">
+        <v>652905050828</v>
+      </c>
+      <c r="H46" t="s">
+        <v>641</v>
+      </c>
+      <c r="I46">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
+        <v>495</v>
+      </c>
+      <c r="B47">
+        <v>2022</v>
+      </c>
+      <c r="C47">
+        <v>12</v>
+      </c>
+      <c r="D47" t="s">
+        <v>512</v>
+      </c>
+      <c r="E47" t="s">
+        <v>505</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>569</v>
+      </c>
+      <c r="G47" s="8">
+        <v>652905060124</v>
+      </c>
+      <c r="H47" t="s">
+        <v>642</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
+        <v>495</v>
+      </c>
+      <c r="B48">
+        <v>2022</v>
+      </c>
+      <c r="C48">
+        <v>12</v>
+      </c>
+      <c r="D48" t="s">
+        <v>512</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>506</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>570</v>
+      </c>
+      <c r="G48" s="8">
+        <v>652905071328</v>
+      </c>
+      <c r="H48" t="s">
+        <v>643</v>
+      </c>
+      <c r="I48">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A49" t="s">
+        <v>495</v>
+      </c>
+      <c r="B49">
+        <v>2022</v>
+      </c>
+      <c r="C49">
+        <v>12</v>
+      </c>
+      <c r="D49" t="s">
+        <v>514</v>
+      </c>
+      <c r="E49" s="9" t="s">
         <v>516</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>527</v>
-      </c>
-      <c r="H2" s="8">
-        <v>652905010112</v>
-      </c>
-      <c r="I2" t="s">
-        <v>603</v>
-      </c>
-      <c r="J2">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>496</v>
-      </c>
-      <c r="B3" t="s">
-        <v>497</v>
-      </c>
-      <c r="C3">
+      <c r="F49" s="12" t="s">
+        <v>571</v>
+      </c>
+      <c r="G49" s="8">
+        <v>652905071717</v>
+      </c>
+      <c r="H49" t="s">
+        <v>644</v>
+      </c>
+      <c r="I49">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A50" t="s">
+        <v>495</v>
+      </c>
+      <c r="B50">
         <v>2022</v>
       </c>
-      <c r="D3">
+      <c r="C50">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D50" t="s">
+        <v>512</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>516</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>572</v>
+      </c>
+      <c r="G50" s="8">
+        <v>652905071724</v>
+      </c>
+      <c r="H50" t="s">
+        <v>644</v>
+      </c>
+      <c r="I50">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A51" t="s">
+        <v>495</v>
+      </c>
+      <c r="B51">
+        <v>2022</v>
+      </c>
+      <c r="C51">
+        <v>12</v>
+      </c>
+      <c r="D51" t="s">
+        <v>512</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>521</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>573</v>
+      </c>
+      <c r="G51" s="8">
+        <v>652905071823</v>
+      </c>
+      <c r="H51" t="s">
+        <v>645</v>
+      </c>
+      <c r="I51">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A52" t="s">
+        <v>495</v>
+      </c>
+      <c r="B52">
+        <v>2022</v>
+      </c>
+      <c r="C52">
+        <v>12</v>
+      </c>
+      <c r="D52" t="s">
+        <v>512</v>
+      </c>
+      <c r="E52" t="s">
+        <v>507</v>
+      </c>
+      <c r="F52" s="12" t="s">
+        <v>574</v>
+      </c>
+      <c r="G52" s="8">
+        <v>652905080122</v>
+      </c>
+      <c r="H52" t="s">
+        <v>646</v>
+      </c>
+      <c r="I52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A53" t="s">
+        <v>495</v>
+      </c>
+      <c r="B53">
+        <v>2022</v>
+      </c>
+      <c r="C53">
+        <v>12</v>
+      </c>
+      <c r="D53" t="s">
+        <v>512</v>
+      </c>
+      <c r="E53" t="s">
+        <v>507</v>
+      </c>
+      <c r="F53" s="12" t="s">
+        <v>575</v>
+      </c>
+      <c r="G53" s="8">
+        <v>652905080221</v>
+      </c>
+      <c r="H53" t="s">
+        <v>647</v>
+      </c>
+      <c r="I53">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A54" t="s">
+        <v>495</v>
+      </c>
+      <c r="B54">
+        <v>2022</v>
+      </c>
+      <c r="C54">
+        <v>12</v>
+      </c>
+      <c r="D54" t="s">
+        <v>512</v>
+      </c>
+      <c r="E54" t="s">
+        <v>507</v>
+      </c>
+      <c r="F54" s="12" t="s">
+        <v>576</v>
+      </c>
+      <c r="G54" s="8">
+        <v>652905080320</v>
+      </c>
+      <c r="H54" t="s">
+        <v>648</v>
+      </c>
+      <c r="I54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A55" t="s">
+        <v>495</v>
+      </c>
+      <c r="B55">
+        <v>2022</v>
+      </c>
+      <c r="C55">
+        <v>12</v>
+      </c>
+      <c r="D55" t="s">
+        <v>512</v>
+      </c>
+      <c r="E55" t="s">
+        <v>508</v>
+      </c>
+      <c r="F55" s="12" t="s">
+        <v>577</v>
+      </c>
+      <c r="G55" s="8">
+        <v>652905090121</v>
+      </c>
+      <c r="H55" t="s">
+        <v>649</v>
+      </c>
+      <c r="I55">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A56" t="s">
+        <v>495</v>
+      </c>
+      <c r="B56">
+        <v>2022</v>
+      </c>
+      <c r="C56">
+        <v>12</v>
+      </c>
+      <c r="D56" t="s">
+        <v>512</v>
+      </c>
+      <c r="E56" t="s">
+        <v>508</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>578</v>
+      </c>
+      <c r="G56" s="8">
+        <v>652905090220</v>
+      </c>
+      <c r="H56" t="s">
+        <v>650</v>
+      </c>
+      <c r="I56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A57" t="s">
+        <v>495</v>
+      </c>
+      <c r="B57">
+        <v>2022</v>
+      </c>
+      <c r="C57">
+        <v>12</v>
+      </c>
+      <c r="D57" t="s">
+        <v>512</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="F57" s="12" t="s">
+        <v>579</v>
+      </c>
+      <c r="G57" s="8">
+        <v>652905100127</v>
+      </c>
+      <c r="H57" t="s">
+        <v>651</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A58" t="s">
+        <v>495</v>
+      </c>
+      <c r="B58">
+        <v>2022</v>
+      </c>
+      <c r="C58">
+        <v>12</v>
+      </c>
+      <c r="D58" t="s">
+        <v>512</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="F58" s="12" t="s">
+        <v>580</v>
+      </c>
+      <c r="G58" s="8">
+        <v>652905100226</v>
+      </c>
+      <c r="H58" t="s">
+        <v>652</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A59" t="s">
+        <v>495</v>
+      </c>
+      <c r="B59">
+        <v>2022</v>
+      </c>
+      <c r="C59">
+        <v>12</v>
+      </c>
+      <c r="D59" t="s">
+        <v>512</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="F59" s="12" t="s">
+        <v>581</v>
+      </c>
+      <c r="G59" s="8">
+        <v>652905100325</v>
+      </c>
+      <c r="H59" t="s">
+        <v>653</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A60" t="s">
+        <v>495</v>
+      </c>
+      <c r="B60">
+        <v>2022</v>
+      </c>
+      <c r="C60">
+        <v>12</v>
+      </c>
+      <c r="D60" t="s">
+        <v>512</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>582</v>
+      </c>
+      <c r="G60" s="8">
+        <v>652905100424</v>
+      </c>
+      <c r="H60" t="s">
+        <v>654</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A61" t="s">
+        <v>495</v>
+      </c>
+      <c r="B61">
+        <v>2022</v>
+      </c>
+      <c r="C61">
+        <v>12</v>
+      </c>
+      <c r="D61" t="s">
+        <v>512</v>
+      </c>
+      <c r="E61" s="11" t="s">
+        <v>509</v>
+      </c>
+      <c r="F61" s="12" t="s">
+        <v>583</v>
+      </c>
+      <c r="G61" s="10">
+        <v>652905100523</v>
+      </c>
+      <c r="H61" t="s">
+        <v>655</v>
+      </c>
+      <c r="I61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A62" t="s">
+        <v>495</v>
+      </c>
+      <c r="B62">
+        <v>2022</v>
+      </c>
+      <c r="C62">
+        <v>12</v>
+      </c>
+      <c r="D62" t="s">
+        <v>512</v>
+      </c>
+      <c r="E62" t="s">
+        <v>510</v>
+      </c>
+      <c r="F62" s="12" t="s">
+        <v>584</v>
+      </c>
+      <c r="G62" s="8">
+        <v>652905110126</v>
+      </c>
+      <c r="H62" t="s">
+        <v>656</v>
+      </c>
+      <c r="I62">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A63" t="s">
+        <v>495</v>
+      </c>
+      <c r="B63">
+        <v>2022</v>
+      </c>
+      <c r="C63">
+        <v>12</v>
+      </c>
+      <c r="D63" t="s">
         <v>514</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>528</v>
-      </c>
-      <c r="H3" s="8">
-        <v>652905010129</v>
-      </c>
-      <c r="I3" t="s">
-        <v>603</v>
-      </c>
-      <c r="J3">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>496</v>
-      </c>
-      <c r="B4" t="s">
-        <v>497</v>
-      </c>
-      <c r="C4">
+      <c r="E63" s="11" t="s">
+        <v>511</v>
+      </c>
+      <c r="F63" s="12" t="s">
+        <v>585</v>
+      </c>
+      <c r="G63" s="10">
+        <v>652905120217</v>
+      </c>
+      <c r="H63" t="s">
+        <v>657</v>
+      </c>
+      <c r="I63">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A64" t="s">
+        <v>495</v>
+      </c>
+      <c r="B64">
         <v>2022</v>
       </c>
-      <c r="D4">
+      <c r="C64">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D64" t="s">
+        <v>512</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>511</v>
+      </c>
+      <c r="F64" s="12" t="s">
+        <v>586</v>
+      </c>
+      <c r="G64" s="10">
+        <v>652905120224</v>
+      </c>
+      <c r="H64" t="s">
+        <v>657</v>
+      </c>
+      <c r="I64">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A65" t="s">
+        <v>495</v>
+      </c>
+      <c r="B65">
+        <v>2022</v>
+      </c>
+      <c r="C65">
+        <v>12</v>
+      </c>
+      <c r="D65" t="s">
+        <v>512</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>511</v>
+      </c>
+      <c r="F65" s="12" t="s">
+        <v>587</v>
+      </c>
+      <c r="G65" s="10">
+        <v>652905120323</v>
+      </c>
+      <c r="H65" t="s">
+        <v>658</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A66" t="s">
+        <v>495</v>
+      </c>
+      <c r="B66">
+        <v>2022</v>
+      </c>
+      <c r="C66">
+        <v>12</v>
+      </c>
+      <c r="D66" t="s">
         <v>514</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>529</v>
-      </c>
-      <c r="H4" s="9">
-        <v>652905010228</v>
-      </c>
-      <c r="I4" t="s">
-        <v>604</v>
-      </c>
-      <c r="J4">
+      <c r="E66" s="11" t="s">
+        <v>511</v>
+      </c>
+      <c r="F66" s="12" t="s">
+        <v>588</v>
+      </c>
+      <c r="G66" s="10">
+        <v>652905120415</v>
+      </c>
+      <c r="H66" t="s">
+        <v>659</v>
+      </c>
+      <c r="I66">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A67" t="s">
+        <v>495</v>
+      </c>
+      <c r="B67">
+        <v>2022</v>
+      </c>
+      <c r="C67">
+        <v>12</v>
+      </c>
+      <c r="D67" t="s">
+        <v>512</v>
+      </c>
+      <c r="E67" s="11" t="s">
+        <v>511</v>
+      </c>
+      <c r="F67" s="12" t="s">
+        <v>589</v>
+      </c>
+      <c r="G67" s="10">
+        <v>652905120422</v>
+      </c>
+      <c r="H67" t="s">
+        <v>659</v>
+      </c>
+      <c r="I67">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A68" t="s">
+        <v>495</v>
+      </c>
+      <c r="B68">
+        <v>2022</v>
+      </c>
+      <c r="C68">
+        <v>12</v>
+      </c>
+      <c r="D68" t="s">
+        <v>512</v>
+      </c>
+      <c r="E68" s="11" t="s">
+        <v>513</v>
+      </c>
+      <c r="F68" s="12" t="s">
+        <v>590</v>
+      </c>
+      <c r="G68" s="10">
+        <v>652905140123</v>
+      </c>
+      <c r="H68" t="s">
+        <v>660</v>
+      </c>
+      <c r="I68">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
-        <v>496</v>
-      </c>
-      <c r="B5" t="s">
-        <v>497</v>
-      </c>
-      <c r="C5">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A69" t="s">
+        <v>495</v>
+      </c>
+      <c r="B69">
         <v>2022</v>
       </c>
-      <c r="D5">
+      <c r="C69">
         <v>12</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D69" t="s">
+        <v>512</v>
+      </c>
+      <c r="E69" s="11" t="s">
+        <v>513</v>
+      </c>
+      <c r="F69" s="12" t="s">
+        <v>591</v>
+      </c>
+      <c r="G69" s="10">
+        <v>652905140222</v>
+      </c>
+      <c r="H69" t="s">
+        <v>661</v>
+      </c>
+      <c r="I69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A70" t="s">
+        <v>495</v>
+      </c>
+      <c r="B70">
+        <v>2022</v>
+      </c>
+      <c r="C70">
+        <v>12</v>
+      </c>
+      <c r="D70" t="s">
+        <v>512</v>
+      </c>
+      <c r="E70" s="11" t="s">
+        <v>513</v>
+      </c>
+      <c r="F70" s="12" t="s">
+        <v>592</v>
+      </c>
+      <c r="G70" s="8">
+        <v>652905140420</v>
+      </c>
+      <c r="H70" t="s">
+        <v>662</v>
+      </c>
+      <c r="I70">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A71" t="s">
+        <v>495</v>
+      </c>
+      <c r="B71">
+        <v>2022</v>
+      </c>
+      <c r="C71">
+        <v>12</v>
+      </c>
+      <c r="D71" t="s">
+        <v>512</v>
+      </c>
+      <c r="E71" s="11" t="s">
+        <v>513</v>
+      </c>
+      <c r="F71" s="12" t="s">
+        <v>593</v>
+      </c>
+      <c r="G71" s="8">
+        <v>652905140628</v>
+      </c>
+      <c r="H71" t="s">
+        <v>663</v>
+      </c>
+      <c r="I71">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A72" t="s">
+        <v>495</v>
+      </c>
+      <c r="B72">
+        <v>2022</v>
+      </c>
+      <c r="C72">
+        <v>12</v>
+      </c>
+      <c r="D72" t="s">
+        <v>512</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>517</v>
+      </c>
+      <c r="F72" s="12" t="s">
+        <v>594</v>
+      </c>
+      <c r="G72" s="8">
+        <v>652905150122</v>
+      </c>
+      <c r="H72" t="s">
+        <v>664</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A73" t="s">
+        <v>495</v>
+      </c>
+      <c r="B73">
+        <v>2022</v>
+      </c>
+      <c r="C73">
+        <v>12</v>
+      </c>
+      <c r="D73" t="s">
+        <v>512</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>518</v>
+      </c>
+      <c r="F73" s="12" t="s">
+        <v>595</v>
+      </c>
+      <c r="G73" s="8">
+        <v>652905160121</v>
+      </c>
+      <c r="H73" t="s">
+        <v>665</v>
+      </c>
+      <c r="I73">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A74" t="s">
+        <v>495</v>
+      </c>
+      <c r="B74">
+        <v>2022</v>
+      </c>
+      <c r="C74">
+        <v>12</v>
+      </c>
+      <c r="D74" t="s">
         <v>514</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>530</v>
-      </c>
-      <c r="H5" s="9">
-        <v>652905010327</v>
-      </c>
-      <c r="I5" t="s">
-        <v>605</v>
-      </c>
-      <c r="J5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>496</v>
-      </c>
-      <c r="B6" t="s">
-        <v>497</v>
-      </c>
-      <c r="C6">
+      <c r="E74" s="9" t="s">
+        <v>518</v>
+      </c>
+      <c r="F74" s="12" t="s">
+        <v>596</v>
+      </c>
+      <c r="G74" s="8">
+        <v>652905160213</v>
+      </c>
+      <c r="H74" t="s">
+        <v>666</v>
+      </c>
+      <c r="I74">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A75" t="s">
+        <v>495</v>
+      </c>
+      <c r="B75">
         <v>2022</v>
       </c>
-      <c r="D6">
+      <c r="C75">
         <v>12</v>
       </c>
-      <c r="E6" t="s">
-        <v>514</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>531</v>
-      </c>
-      <c r="H6" s="9">
-        <v>652905010426</v>
-      </c>
-      <c r="I6" t="s">
-        <v>606</v>
-      </c>
-      <c r="J6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
-        <v>496</v>
-      </c>
-      <c r="B7" t="s">
-        <v>497</v>
-      </c>
-      <c r="C7">
+      <c r="D75" t="s">
+        <v>512</v>
+      </c>
+      <c r="E75" s="9" t="s">
+        <v>518</v>
+      </c>
+      <c r="F75" s="12" t="s">
+        <v>597</v>
+      </c>
+      <c r="G75" s="8">
+        <v>652905160220</v>
+      </c>
+      <c r="H75" t="s">
+        <v>666</v>
+      </c>
+      <c r="I75">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A76" t="s">
+        <v>495</v>
+      </c>
+      <c r="B76">
         <v>2022</v>
       </c>
-      <c r="D7">
+      <c r="C76">
         <v>12</v>
       </c>
-      <c r="E7" t="s">
-        <v>516</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>499</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>532</v>
-      </c>
-      <c r="H7" s="9">
-        <v>652905010518</v>
-      </c>
-      <c r="I7" t="s">
-        <v>607</v>
-      </c>
-      <c r="J7">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>496</v>
-      </c>
-      <c r="B8" t="s">
-        <v>497</v>
-      </c>
-      <c r="C8">
+      <c r="D76" t="s">
+        <v>512</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>520</v>
+      </c>
+      <c r="F76" s="12" t="s">
+        <v>598</v>
+      </c>
+      <c r="G76" s="8">
+        <v>652905170120</v>
+      </c>
+      <c r="H76" t="s">
+        <v>667</v>
+      </c>
+      <c r="I76">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A77" t="s">
+        <v>495</v>
+      </c>
+      <c r="B77">
         <v>2022</v>
       </c>
-      <c r="D8">
+      <c r="C77">
         <v>12</v>
       </c>
-      <c r="E8" t="s">
-        <v>514</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>499</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>533</v>
-      </c>
-      <c r="H8" s="9">
-        <v>652905010525</v>
-      </c>
-      <c r="I8" t="s">
-        <v>607</v>
-      </c>
-      <c r="J8">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>496</v>
-      </c>
-      <c r="B9" t="s">
-        <v>497</v>
-      </c>
-      <c r="C9">
-        <v>2022</v>
-      </c>
-      <c r="D9">
-        <v>12</v>
-      </c>
-      <c r="E9" t="s">
-        <v>514</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>534</v>
-      </c>
-      <c r="H9" s="9">
-        <v>652905010624</v>
-      </c>
-      <c r="I9" t="s">
-        <v>608</v>
-      </c>
-      <c r="J9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
-        <v>496</v>
-      </c>
-      <c r="B10" t="s">
-        <v>497</v>
-      </c>
-      <c r="C10">
-        <v>2022</v>
-      </c>
-      <c r="D10">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
-        <v>514</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>535</v>
-      </c>
-      <c r="H10" s="9">
-        <v>652905010723</v>
-      </c>
-      <c r="I10" t="s">
-        <v>609</v>
-      </c>
-      <c r="J10">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
-        <v>496</v>
-      </c>
-      <c r="B11" t="s">
-        <v>497</v>
-      </c>
-      <c r="C11">
-        <v>2022</v>
-      </c>
-      <c r="D11">
-        <v>12</v>
-      </c>
-      <c r="E11" t="s">
-        <v>514</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>536</v>
-      </c>
-      <c r="H11" s="9">
-        <v>652905010822</v>
-      </c>
-      <c r="I11" t="s">
-        <v>610</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
-        <v>496</v>
-      </c>
-      <c r="B12" t="s">
-        <v>497</v>
-      </c>
-      <c r="C12">
-        <v>2022</v>
-      </c>
-      <c r="D12">
-        <v>12</v>
-      </c>
-      <c r="E12" t="s">
-        <v>514</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>537</v>
-      </c>
-      <c r="H12" s="9">
-        <v>652905010914</v>
-      </c>
-      <c r="I12" t="s">
-        <v>611</v>
-      </c>
-      <c r="J12">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
-        <v>496</v>
-      </c>
-      <c r="B13" t="s">
-        <v>517</v>
-      </c>
-      <c r="C13">
-        <v>2022</v>
-      </c>
-      <c r="D13">
-        <v>12</v>
-      </c>
-      <c r="E13" t="s">
-        <v>514</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>538</v>
-      </c>
-      <c r="H13" s="9">
-        <v>652905010921</v>
-      </c>
-      <c r="I13" t="s">
-        <v>611</v>
-      </c>
-      <c r="J13">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
-        <v>496</v>
-      </c>
-      <c r="B14" t="s">
-        <v>497</v>
-      </c>
-      <c r="C14">
-        <v>2022</v>
-      </c>
-      <c r="D14">
-        <v>12</v>
-      </c>
-      <c r="E14" t="s">
-        <v>514</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>539</v>
-      </c>
-      <c r="H14" s="9">
-        <v>652905011126</v>
-      </c>
-      <c r="I14" t="s">
-        <v>612</v>
-      </c>
-      <c r="J14">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A15" t="s">
-        <v>496</v>
-      </c>
-      <c r="B15" t="s">
-        <v>497</v>
-      </c>
-      <c r="C15">
-        <v>2022</v>
-      </c>
-      <c r="D15">
-        <v>12</v>
-      </c>
-      <c r="E15" t="s">
-        <v>514</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>540</v>
-      </c>
-      <c r="H15" s="9">
-        <v>652905011225</v>
-      </c>
-      <c r="I15" t="s">
-        <v>613</v>
-      </c>
-      <c r="J15">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
-        <v>496</v>
-      </c>
-      <c r="B16" t="s">
-        <v>497</v>
-      </c>
-      <c r="C16">
-        <v>2022</v>
-      </c>
-      <c r="D16">
-        <v>12</v>
-      </c>
-      <c r="E16" t="s">
-        <v>514</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>541</v>
-      </c>
-      <c r="H16" s="9">
-        <v>652905011324</v>
-      </c>
-      <c r="I16" t="s">
-        <v>614</v>
-      </c>
-      <c r="J16">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
-        <v>496</v>
-      </c>
-      <c r="B17" t="s">
-        <v>497</v>
-      </c>
-      <c r="C17">
-        <v>2022</v>
-      </c>
-      <c r="D17">
-        <v>12</v>
-      </c>
-      <c r="E17" t="s">
-        <v>514</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>542</v>
-      </c>
-      <c r="H17" s="9">
-        <v>652905011423</v>
-      </c>
-      <c r="I17" t="s">
-        <v>615</v>
-      </c>
-      <c r="J17">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
-        <v>496</v>
-      </c>
-      <c r="B18" t="s">
-        <v>497</v>
-      </c>
-      <c r="C18">
-        <v>2022</v>
-      </c>
-      <c r="D18">
-        <v>12</v>
-      </c>
-      <c r="E18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>543</v>
-      </c>
-      <c r="H18" s="9">
-        <v>652905011522</v>
-      </c>
-      <c r="I18" t="s">
-        <v>616</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
-        <v>496</v>
-      </c>
-      <c r="B19" t="s">
-        <v>497</v>
-      </c>
-      <c r="C19">
-        <v>2022</v>
-      </c>
-      <c r="D19">
-        <v>12</v>
-      </c>
-      <c r="E19" t="s">
-        <v>514</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>500</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>544</v>
-      </c>
-      <c r="H19" s="9">
-        <v>652905020128</v>
-      </c>
-      <c r="I19" t="s">
-        <v>617</v>
-      </c>
-      <c r="J19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A20" t="s">
-        <v>496</v>
-      </c>
-      <c r="B20" t="s">
-        <v>497</v>
-      </c>
-      <c r="C20">
-        <v>2022</v>
-      </c>
-      <c r="D20">
-        <v>12</v>
-      </c>
-      <c r="E20" t="s">
-        <v>514</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>500</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>545</v>
-      </c>
-      <c r="H20" s="9">
-        <v>652905020227</v>
-      </c>
-      <c r="I20" t="s">
-        <v>618</v>
-      </c>
-      <c r="J20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
-        <v>496</v>
-      </c>
-      <c r="B21" t="s">
-        <v>497</v>
-      </c>
-      <c r="C21">
-        <v>2022</v>
-      </c>
-      <c r="D21">
-        <v>12</v>
-      </c>
-      <c r="E21" t="s">
-        <v>514</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>500</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>546</v>
-      </c>
-      <c r="H21" s="9">
-        <v>652905020326</v>
-      </c>
-      <c r="I21" t="s">
-        <v>619</v>
-      </c>
-      <c r="J21">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A22" t="s">
-        <v>496</v>
-      </c>
-      <c r="B22" t="s">
-        <v>497</v>
-      </c>
-      <c r="C22">
-        <v>2022</v>
-      </c>
-      <c r="D22">
-        <v>12</v>
-      </c>
-      <c r="E22" t="s">
-        <v>514</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>500</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>547</v>
-      </c>
-      <c r="H22" s="9">
-        <v>652905020425</v>
-      </c>
-      <c r="I22" t="s">
-        <v>620</v>
-      </c>
-      <c r="J22">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
-        <v>496</v>
-      </c>
-      <c r="B23" t="s">
-        <v>497</v>
-      </c>
-      <c r="C23">
-        <v>2022</v>
-      </c>
-      <c r="D23">
-        <v>12</v>
-      </c>
-      <c r="E23" t="s">
-        <v>514</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>500</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>548</v>
-      </c>
-      <c r="H23" s="9">
-        <v>652905020623</v>
-      </c>
-      <c r="I23" t="s">
-        <v>621</v>
-      </c>
-      <c r="J23">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A24" t="s">
-        <v>496</v>
-      </c>
-      <c r="B24" t="s">
-        <v>497</v>
-      </c>
-      <c r="C24">
-        <v>2022</v>
-      </c>
-      <c r="D24">
-        <v>12</v>
-      </c>
-      <c r="E24" t="s">
-        <v>514</v>
-      </c>
-      <c r="F24" t="s">
-        <v>501</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>549</v>
-      </c>
-      <c r="H24" s="9">
-        <v>652905030127</v>
-      </c>
-      <c r="I24" t="s">
-        <v>622</v>
-      </c>
-      <c r="J24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
-        <v>496</v>
-      </c>
-      <c r="B25" t="s">
-        <v>497</v>
-      </c>
-      <c r="C25">
-        <v>2022</v>
-      </c>
-      <c r="D25">
-        <v>12</v>
-      </c>
-      <c r="E25" t="s">
-        <v>514</v>
-      </c>
-      <c r="F25" t="s">
-        <v>501</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>550</v>
-      </c>
-      <c r="H25" s="9">
-        <v>652905030226</v>
-      </c>
-      <c r="I25" t="s">
-        <v>623</v>
-      </c>
-      <c r="J25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A26" t="s">
-        <v>496</v>
-      </c>
-      <c r="B26" t="s">
-        <v>497</v>
-      </c>
-      <c r="C26">
-        <v>2022</v>
-      </c>
-      <c r="D26">
-        <v>12</v>
-      </c>
-      <c r="E26" t="s">
-        <v>514</v>
-      </c>
-      <c r="F26" t="s">
-        <v>502</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>551</v>
-      </c>
-      <c r="H26" s="9">
-        <v>652905030325</v>
-      </c>
-      <c r="I26" t="s">
-        <v>624</v>
-      </c>
-      <c r="J26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A27" t="s">
-        <v>496</v>
-      </c>
-      <c r="B27" t="s">
-        <v>497</v>
-      </c>
-      <c r="C27">
-        <v>2022</v>
-      </c>
-      <c r="D27">
-        <v>12</v>
-      </c>
-      <c r="E27" t="s">
-        <v>514</v>
-      </c>
-      <c r="F27" t="s">
-        <v>502</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>552</v>
-      </c>
-      <c r="H27" s="9">
-        <v>652905030424</v>
-      </c>
-      <c r="I27" t="s">
-        <v>625</v>
-      </c>
-      <c r="J27">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A28" t="s">
-        <v>496</v>
-      </c>
-      <c r="B28" t="s">
-        <v>497</v>
-      </c>
-      <c r="C28">
-        <v>2022</v>
-      </c>
-      <c r="D28">
-        <v>12</v>
-      </c>
-      <c r="E28" t="s">
-        <v>514</v>
-      </c>
-      <c r="F28" t="s">
-        <v>522</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>553</v>
-      </c>
-      <c r="H28" s="9">
-        <v>652905030523</v>
-      </c>
-      <c r="I28" t="s">
-        <v>626</v>
-      </c>
-      <c r="J28">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A29" t="s">
-        <v>496</v>
-      </c>
-      <c r="B29" t="s">
-        <v>497</v>
-      </c>
-      <c r="C29">
-        <v>2022</v>
-      </c>
-      <c r="D29">
-        <v>12</v>
-      </c>
-      <c r="E29" t="s">
-        <v>514</v>
-      </c>
-      <c r="F29" t="s">
-        <v>525</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>554</v>
-      </c>
-      <c r="H29" s="9">
-        <v>652905030622</v>
-      </c>
-      <c r="I29" t="s">
-        <v>627</v>
-      </c>
-      <c r="J29">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A30" t="s">
-        <v>496</v>
-      </c>
-      <c r="B30" t="s">
-        <v>497</v>
-      </c>
-      <c r="C30">
-        <v>2022</v>
-      </c>
-      <c r="D30">
-        <v>12</v>
-      </c>
-      <c r="E30" t="s">
-        <v>514</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>503</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>555</v>
-      </c>
-      <c r="H30" s="9">
-        <v>652905040126</v>
-      </c>
-      <c r="I30" t="s">
-        <v>628</v>
-      </c>
-      <c r="J30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A31" t="s">
-        <v>496</v>
-      </c>
-      <c r="B31" t="s">
-        <v>497</v>
-      </c>
-      <c r="C31">
-        <v>2022</v>
-      </c>
-      <c r="D31">
-        <v>12</v>
-      </c>
-      <c r="E31" t="s">
-        <v>514</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>503</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>556</v>
-      </c>
-      <c r="H31" s="9">
-        <v>652905040225</v>
-      </c>
-      <c r="I31" t="s">
-        <v>629</v>
-      </c>
-      <c r="J31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A32" t="s">
-        <v>496</v>
-      </c>
-      <c r="B32" t="s">
-        <v>497</v>
-      </c>
-      <c r="C32">
-        <v>2022</v>
-      </c>
-      <c r="D32">
-        <v>12</v>
-      </c>
-      <c r="E32" t="s">
-        <v>514</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>504</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>557</v>
-      </c>
-      <c r="H32" s="9">
-        <v>652905040324</v>
-      </c>
-      <c r="I32" t="s">
-        <v>630</v>
-      </c>
-      <c r="J32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A33" t="s">
-        <v>496</v>
-      </c>
-      <c r="B33" t="s">
-        <v>497</v>
-      </c>
-      <c r="C33">
-        <v>2022</v>
-      </c>
-      <c r="D33">
-        <v>12</v>
-      </c>
-      <c r="E33" t="s">
-        <v>514</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>503</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>558</v>
-      </c>
-      <c r="H33" s="9">
-        <v>652905040423</v>
-      </c>
-      <c r="I33" t="s">
-        <v>631</v>
-      </c>
-      <c r="J33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A34" t="s">
-        <v>496</v>
-      </c>
-      <c r="B34" t="s">
-        <v>497</v>
-      </c>
-      <c r="C34">
-        <v>2022</v>
-      </c>
-      <c r="D34">
-        <v>12</v>
-      </c>
-      <c r="E34" t="s">
-        <v>514</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>505</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>559</v>
-      </c>
-      <c r="H34" s="9">
-        <v>652905040522</v>
-      </c>
-      <c r="I34" t="s">
-        <v>632</v>
-      </c>
-      <c r="J34">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A35" t="s">
-        <v>496</v>
-      </c>
-      <c r="B35" t="s">
-        <v>497</v>
-      </c>
-      <c r="C35">
-        <v>2022</v>
-      </c>
-      <c r="D35">
-        <v>12</v>
-      </c>
-      <c r="E35" t="s">
-        <v>514</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>503</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>560</v>
-      </c>
-      <c r="H35" s="11">
-        <v>652905040621</v>
-      </c>
-      <c r="I35" t="s">
-        <v>633</v>
-      </c>
-      <c r="J35">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A36" t="s">
-        <v>496</v>
-      </c>
-      <c r="B36" t="s">
-        <v>497</v>
-      </c>
-      <c r="C36">
-        <v>2022</v>
-      </c>
-      <c r="D36">
-        <v>12</v>
-      </c>
-      <c r="E36" t="s">
-        <v>514</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>503</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>561</v>
-      </c>
-      <c r="H36" s="11">
-        <v>652905040720</v>
-      </c>
-      <c r="I36" t="s">
-        <v>634</v>
-      </c>
-      <c r="J36">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A37" t="s">
-        <v>496</v>
-      </c>
-      <c r="B37" t="s">
-        <v>497</v>
-      </c>
-      <c r="C37">
-        <v>2022</v>
-      </c>
-      <c r="D37">
-        <v>12</v>
-      </c>
-      <c r="E37" t="s">
-        <v>514</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>503</v>
-      </c>
-      <c r="G37" s="7" t="s">
-        <v>562</v>
-      </c>
-      <c r="H37" s="11">
-        <v>652905040836</v>
-      </c>
-      <c r="I37" t="s">
-        <v>635</v>
-      </c>
-      <c r="J37">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A38" t="s">
-        <v>496</v>
-      </c>
-      <c r="B38" t="s">
-        <v>497</v>
-      </c>
-      <c r="C38">
-        <v>2022</v>
-      </c>
-      <c r="D38">
-        <v>12</v>
-      </c>
-      <c r="E38" t="s">
-        <v>514</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>518</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>563</v>
-      </c>
-      <c r="H38" s="11">
-        <v>652905040928</v>
-      </c>
-      <c r="I38" t="s">
-        <v>636</v>
-      </c>
-      <c r="J38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A39" t="s">
-        <v>496</v>
-      </c>
-      <c r="B39" t="s">
-        <v>497</v>
-      </c>
-      <c r="C39">
-        <v>2022</v>
-      </c>
-      <c r="D39">
-        <v>12</v>
-      </c>
-      <c r="E39" t="s">
-        <v>514</v>
-      </c>
-      <c r="F39" s="10" t="s">
-        <v>506</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>564</v>
-      </c>
-      <c r="H39" s="9">
-        <v>652905050125</v>
-      </c>
-      <c r="I39" t="s">
-        <v>637</v>
-      </c>
-      <c r="J39">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A40" t="s">
-        <v>496</v>
-      </c>
-      <c r="B40" t="s">
-        <v>497</v>
-      </c>
-      <c r="C40">
-        <v>2022</v>
-      </c>
-      <c r="D40">
-        <v>12</v>
-      </c>
-      <c r="E40" t="s">
-        <v>514</v>
-      </c>
-      <c r="F40" s="10" t="s">
-        <v>506</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>565</v>
-      </c>
-      <c r="H40" s="9">
-        <v>652905050224</v>
-      </c>
-      <c r="I40" t="s">
-        <v>638</v>
-      </c>
-      <c r="J40">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A41" t="s">
-        <v>496</v>
-      </c>
-      <c r="B41" t="s">
-        <v>497</v>
-      </c>
-      <c r="C41">
-        <v>2022</v>
-      </c>
-      <c r="D41">
-        <v>12</v>
-      </c>
-      <c r="E41" t="s">
-        <v>514</v>
-      </c>
-      <c r="F41" s="10" t="s">
-        <v>506</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>566</v>
-      </c>
-      <c r="H41" s="9">
-        <v>652905050323</v>
-      </c>
-      <c r="I41" t="s">
-        <v>639</v>
-      </c>
-      <c r="J41">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A42" t="s">
-        <v>496</v>
-      </c>
-      <c r="B42" t="s">
-        <v>497</v>
-      </c>
-      <c r="C42">
-        <v>2022</v>
-      </c>
-      <c r="D42">
-        <v>12</v>
-      </c>
-      <c r="E42" t="s">
-        <v>514</v>
-      </c>
-      <c r="F42" s="10" t="s">
-        <v>506</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>567</v>
-      </c>
-      <c r="H42" s="9">
-        <v>652905050422</v>
-      </c>
-      <c r="I42" t="s">
-        <v>640</v>
-      </c>
-      <c r="J42">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A43" t="s">
-        <v>496</v>
-      </c>
-      <c r="B43" t="s">
-        <v>497</v>
-      </c>
-      <c r="C43">
-        <v>2022</v>
-      </c>
-      <c r="D43">
-        <v>12</v>
-      </c>
-      <c r="E43" t="s">
-        <v>514</v>
-      </c>
-      <c r="F43" s="10" t="s">
-        <v>506</v>
-      </c>
-      <c r="G43" s="7" t="s">
-        <v>568</v>
-      </c>
-      <c r="H43" s="11">
-        <v>652905050521</v>
-      </c>
-      <c r="I43" t="s">
-        <v>641</v>
-      </c>
-      <c r="J43">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A44" t="s">
-        <v>496</v>
-      </c>
-      <c r="B44" t="s">
-        <v>497</v>
-      </c>
-      <c r="C44">
-        <v>2022</v>
-      </c>
-      <c r="D44">
-        <v>12</v>
-      </c>
-      <c r="E44" t="s">
-        <v>514</v>
-      </c>
-      <c r="F44" s="10" t="s">
-        <v>506</v>
-      </c>
-      <c r="G44" s="7" t="s">
-        <v>569</v>
-      </c>
-      <c r="H44" s="11">
-        <v>652905050620</v>
-      </c>
-      <c r="I44" t="s">
-        <v>642</v>
-      </c>
-      <c r="J44">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A45" t="s">
-        <v>496</v>
-      </c>
-      <c r="B45" t="s">
-        <v>497</v>
-      </c>
-      <c r="C45">
-        <v>2022</v>
-      </c>
-      <c r="D45">
-        <v>12</v>
-      </c>
-      <c r="E45" t="s">
-        <v>514</v>
-      </c>
-      <c r="F45" s="10" t="s">
-        <v>506</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>570</v>
-      </c>
-      <c r="H45" s="11">
-        <v>652905050729</v>
-      </c>
-      <c r="I45" t="s">
-        <v>643</v>
-      </c>
-      <c r="J45">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A46" t="s">
-        <v>496</v>
-      </c>
-      <c r="B46" t="s">
-        <v>497</v>
-      </c>
-      <c r="C46">
-        <v>2022</v>
-      </c>
-      <c r="D46">
-        <v>12</v>
-      </c>
-      <c r="E46" t="s">
-        <v>514</v>
-      </c>
-      <c r="F46" s="10" t="s">
-        <v>506</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>571</v>
-      </c>
-      <c r="H46" s="11">
-        <v>652905050828</v>
-      </c>
-      <c r="I46" t="s">
-        <v>644</v>
-      </c>
-      <c r="J46">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A47" t="s">
-        <v>496</v>
-      </c>
-      <c r="B47" t="s">
-        <v>497</v>
-      </c>
-      <c r="C47">
-        <v>2022</v>
-      </c>
-      <c r="D47">
-        <v>12</v>
-      </c>
-      <c r="E47" t="s">
-        <v>514</v>
-      </c>
-      <c r="F47" t="s">
-        <v>507</v>
-      </c>
-      <c r="G47" s="7" t="s">
-        <v>572</v>
-      </c>
-      <c r="H47" s="9">
-        <v>652905060124</v>
-      </c>
-      <c r="I47" t="s">
-        <v>645</v>
-      </c>
-      <c r="J47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A48" t="s">
-        <v>496</v>
-      </c>
-      <c r="B48" t="s">
-        <v>497</v>
-      </c>
-      <c r="C48">
-        <v>2022</v>
-      </c>
-      <c r="D48">
-        <v>12</v>
-      </c>
-      <c r="E48" t="s">
-        <v>514</v>
-      </c>
-      <c r="F48" s="12" t="s">
-        <v>508</v>
-      </c>
-      <c r="G48" s="7" t="s">
-        <v>573</v>
-      </c>
-      <c r="H48" s="9">
-        <v>652905071328</v>
-      </c>
-      <c r="I48" t="s">
-        <v>646</v>
-      </c>
-      <c r="J48">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A49" t="s">
-        <v>496</v>
-      </c>
-      <c r="B49" t="s">
-        <v>497</v>
-      </c>
-      <c r="C49">
-        <v>2022</v>
-      </c>
-      <c r="D49">
-        <v>12</v>
-      </c>
-      <c r="E49" t="s">
-        <v>516</v>
-      </c>
-      <c r="F49" s="10" t="s">
-        <v>519</v>
-      </c>
-      <c r="G49" s="7" t="s">
-        <v>574</v>
-      </c>
-      <c r="H49" s="9">
-        <v>652905071717</v>
-      </c>
-      <c r="I49" t="s">
-        <v>647</v>
-      </c>
-      <c r="J49">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A50" t="s">
-        <v>496</v>
-      </c>
-      <c r="B50" t="s">
-        <v>497</v>
-      </c>
-      <c r="C50">
-        <v>2022</v>
-      </c>
-      <c r="D50">
-        <v>12</v>
-      </c>
-      <c r="E50" t="s">
-        <v>514</v>
-      </c>
-      <c r="F50" s="10" t="s">
-        <v>519</v>
-      </c>
-      <c r="G50" s="7" t="s">
-        <v>575</v>
-      </c>
-      <c r="H50" s="9">
-        <v>652905071724</v>
-      </c>
-      <c r="I50" t="s">
-        <v>647</v>
-      </c>
-      <c r="J50">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A51" t="s">
-        <v>496</v>
-      </c>
-      <c r="B51" t="s">
-        <v>497</v>
-      </c>
-      <c r="C51">
-        <v>2022</v>
-      </c>
-      <c r="D51">
-        <v>12</v>
-      </c>
-      <c r="E51" t="s">
-        <v>514</v>
-      </c>
-      <c r="F51" s="10" t="s">
-        <v>524</v>
-      </c>
-      <c r="G51" s="7" t="s">
-        <v>576</v>
-      </c>
-      <c r="H51" s="9">
-        <v>652905071823</v>
-      </c>
-      <c r="I51" t="s">
-        <v>648</v>
-      </c>
-      <c r="J51">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A52" t="s">
-        <v>496</v>
-      </c>
-      <c r="B52" t="s">
-        <v>497</v>
-      </c>
-      <c r="C52">
-        <v>2022</v>
-      </c>
-      <c r="D52">
-        <v>12</v>
-      </c>
-      <c r="E52" t="s">
-        <v>514</v>
-      </c>
-      <c r="F52" t="s">
-        <v>509</v>
-      </c>
-      <c r="G52" s="7" t="s">
-        <v>577</v>
-      </c>
-      <c r="H52" s="9">
-        <v>652905080122</v>
-      </c>
-      <c r="I52" t="s">
-        <v>649</v>
-      </c>
-      <c r="J52">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A53" t="s">
-        <v>496</v>
-      </c>
-      <c r="B53" t="s">
-        <v>497</v>
-      </c>
-      <c r="C53">
-        <v>2022</v>
-      </c>
-      <c r="D53">
-        <v>12</v>
-      </c>
-      <c r="E53" t="s">
-        <v>514</v>
-      </c>
-      <c r="F53" t="s">
-        <v>509</v>
-      </c>
-      <c r="G53" s="7" t="s">
-        <v>578</v>
-      </c>
-      <c r="H53" s="9">
-        <v>652905080221</v>
-      </c>
-      <c r="I53" t="s">
-        <v>650</v>
-      </c>
-      <c r="J53">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A54" t="s">
-        <v>496</v>
-      </c>
-      <c r="B54" t="s">
-        <v>497</v>
-      </c>
-      <c r="C54">
-        <v>2022</v>
-      </c>
-      <c r="D54">
-        <v>12</v>
-      </c>
-      <c r="E54" t="s">
-        <v>514</v>
-      </c>
-      <c r="F54" t="s">
-        <v>509</v>
-      </c>
-      <c r="G54" s="7" t="s">
-        <v>579</v>
-      </c>
-      <c r="H54" s="9">
-        <v>652905080320</v>
-      </c>
-      <c r="I54" t="s">
-        <v>651</v>
-      </c>
-      <c r="J54">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A55" t="s">
-        <v>496</v>
-      </c>
-      <c r="B55" t="s">
-        <v>497</v>
-      </c>
-      <c r="C55">
-        <v>2022</v>
-      </c>
-      <c r="D55">
-        <v>12</v>
-      </c>
-      <c r="E55" t="s">
-        <v>514</v>
-      </c>
-      <c r="F55" t="s">
-        <v>510</v>
-      </c>
-      <c r="G55" s="7" t="s">
-        <v>580</v>
-      </c>
-      <c r="H55" s="9">
-        <v>652905090121</v>
-      </c>
-      <c r="I55" t="s">
-        <v>652</v>
-      </c>
-      <c r="J55">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A56" t="s">
-        <v>496</v>
-      </c>
-      <c r="B56" t="s">
-        <v>497</v>
-      </c>
-      <c r="C56">
-        <v>2022</v>
-      </c>
-      <c r="D56">
-        <v>12</v>
-      </c>
-      <c r="E56" t="s">
-        <v>514</v>
-      </c>
-      <c r="F56" t="s">
-        <v>510</v>
-      </c>
-      <c r="G56" s="7" t="s">
-        <v>581</v>
-      </c>
-      <c r="H56" s="9">
-        <v>652905090220</v>
-      </c>
-      <c r="I56" t="s">
-        <v>653</v>
-      </c>
-      <c r="J56">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A57" t="s">
-        <v>496</v>
-      </c>
-      <c r="B57" t="s">
-        <v>497</v>
-      </c>
-      <c r="C57">
-        <v>2022</v>
-      </c>
-      <c r="D57">
-        <v>12</v>
-      </c>
-      <c r="E57" t="s">
-        <v>514</v>
-      </c>
-      <c r="F57" s="10" t="s">
-        <v>511</v>
-      </c>
-      <c r="G57" s="7" t="s">
-        <v>582</v>
-      </c>
-      <c r="H57" s="9">
-        <v>652905100127</v>
-      </c>
-      <c r="I57" t="s">
-        <v>654</v>
-      </c>
-      <c r="J57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A58" t="s">
-        <v>496</v>
-      </c>
-      <c r="B58" t="s">
-        <v>497</v>
-      </c>
-      <c r="C58">
-        <v>2022</v>
-      </c>
-      <c r="D58">
-        <v>12</v>
-      </c>
-      <c r="E58" t="s">
-        <v>514</v>
-      </c>
-      <c r="F58" s="10" t="s">
-        <v>511</v>
-      </c>
-      <c r="G58" s="7" t="s">
-        <v>583</v>
-      </c>
-      <c r="H58" s="9">
-        <v>652905100226</v>
-      </c>
-      <c r="I58" t="s">
-        <v>655</v>
-      </c>
-      <c r="J58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A59" t="s">
-        <v>496</v>
-      </c>
-      <c r="B59" t="s">
-        <v>497</v>
-      </c>
-      <c r="C59">
-        <v>2022</v>
-      </c>
-      <c r="D59">
-        <v>12</v>
-      </c>
-      <c r="E59" t="s">
-        <v>514</v>
-      </c>
-      <c r="F59" s="10" t="s">
-        <v>511</v>
-      </c>
-      <c r="G59" s="7" t="s">
-        <v>584</v>
-      </c>
-      <c r="H59" s="9">
-        <v>652905100325</v>
-      </c>
-      <c r="I59" t="s">
-        <v>656</v>
-      </c>
-      <c r="J59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A60" t="s">
-        <v>496</v>
-      </c>
-      <c r="B60" t="s">
-        <v>497</v>
-      </c>
-      <c r="C60">
-        <v>2022</v>
-      </c>
-      <c r="D60">
-        <v>12</v>
-      </c>
-      <c r="E60" t="s">
-        <v>514</v>
-      </c>
-      <c r="F60" s="10" t="s">
-        <v>511</v>
-      </c>
-      <c r="G60" s="7" t="s">
-        <v>585</v>
-      </c>
-      <c r="H60" s="9">
-        <v>652905100424</v>
-      </c>
-      <c r="I60" t="s">
-        <v>657</v>
-      </c>
-      <c r="J60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A61" t="s">
-        <v>496</v>
-      </c>
-      <c r="B61" t="s">
-        <v>497</v>
-      </c>
-      <c r="C61">
-        <v>2022</v>
-      </c>
-      <c r="D61">
-        <v>12</v>
-      </c>
-      <c r="E61" t="s">
-        <v>514</v>
-      </c>
-      <c r="F61" s="12" t="s">
-        <v>511</v>
-      </c>
-      <c r="G61" s="7" t="s">
-        <v>586</v>
-      </c>
-      <c r="H61" s="11">
-        <v>652905100523</v>
-      </c>
-      <c r="I61" t="s">
-        <v>658</v>
-      </c>
-      <c r="J61">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A62" t="s">
-        <v>496</v>
-      </c>
-      <c r="B62" t="s">
-        <v>497</v>
-      </c>
-      <c r="C62">
-        <v>2022</v>
-      </c>
-      <c r="D62">
-        <v>12</v>
-      </c>
-      <c r="E62" t="s">
-        <v>514</v>
-      </c>
-      <c r="F62" t="s">
+      <c r="D77" t="s">
         <v>512</v>
       </c>
-      <c r="G62" s="7" t="s">
-        <v>587</v>
-      </c>
-      <c r="H62" s="9">
-        <v>652905110126</v>
-      </c>
-      <c r="I62" t="s">
-        <v>659</v>
-      </c>
-      <c r="J62">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A63" t="s">
-        <v>496</v>
-      </c>
-      <c r="B63" t="s">
-        <v>497</v>
-      </c>
-      <c r="C63">
-        <v>2022</v>
-      </c>
-      <c r="D63">
-        <v>12</v>
-      </c>
-      <c r="E63" t="s">
-        <v>516</v>
-      </c>
-      <c r="F63" s="12" t="s">
-        <v>513</v>
-      </c>
-      <c r="G63" s="7" t="s">
-        <v>588</v>
-      </c>
-      <c r="H63" s="11">
-        <v>652905120217</v>
-      </c>
-      <c r="I63" t="s">
-        <v>660</v>
-      </c>
-      <c r="J63">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A64" t="s">
-        <v>496</v>
-      </c>
-      <c r="B64" t="s">
-        <v>497</v>
-      </c>
-      <c r="C64">
-        <v>2022</v>
-      </c>
-      <c r="D64">
-        <v>12</v>
-      </c>
-      <c r="E64" t="s">
-        <v>514</v>
-      </c>
-      <c r="F64" s="12" t="s">
-        <v>513</v>
-      </c>
-      <c r="G64" s="7" t="s">
-        <v>589</v>
-      </c>
-      <c r="H64" s="11">
-        <v>652905120224</v>
-      </c>
-      <c r="I64" t="s">
-        <v>660</v>
-      </c>
-      <c r="J64">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A65" t="s">
-        <v>496</v>
-      </c>
-      <c r="B65" t="s">
-        <v>497</v>
-      </c>
-      <c r="C65">
-        <v>2022</v>
-      </c>
-      <c r="D65">
-        <v>12</v>
-      </c>
-      <c r="E65" t="s">
-        <v>514</v>
-      </c>
-      <c r="F65" s="12" t="s">
-        <v>513</v>
-      </c>
-      <c r="G65" s="7" t="s">
-        <v>590</v>
-      </c>
-      <c r="H65" s="11">
-        <v>652905120323</v>
-      </c>
-      <c r="I65" t="s">
-        <v>661</v>
-      </c>
-      <c r="J65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A66" t="s">
-        <v>496</v>
-      </c>
-      <c r="B66" t="s">
-        <v>497</v>
-      </c>
-      <c r="C66">
-        <v>2022</v>
-      </c>
-      <c r="D66">
-        <v>12</v>
-      </c>
-      <c r="E66" t="s">
-        <v>516</v>
-      </c>
-      <c r="F66" s="12" t="s">
-        <v>513</v>
-      </c>
-      <c r="G66" s="7" t="s">
-        <v>591</v>
-      </c>
-      <c r="H66" s="11">
-        <v>652905120415</v>
-      </c>
-      <c r="I66" t="s">
-        <v>662</v>
-      </c>
-      <c r="J66">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A67" t="s">
-        <v>496</v>
-      </c>
-      <c r="B67" t="s">
-        <v>497</v>
-      </c>
-      <c r="C67">
-        <v>2022</v>
-      </c>
-      <c r="D67">
-        <v>12</v>
-      </c>
-      <c r="E67" t="s">
-        <v>514</v>
-      </c>
-      <c r="F67" s="12" t="s">
-        <v>513</v>
-      </c>
-      <c r="G67" s="7" t="s">
-        <v>592</v>
-      </c>
-      <c r="H67" s="11">
-        <v>652905120422</v>
-      </c>
-      <c r="I67" t="s">
-        <v>662</v>
-      </c>
-      <c r="J67">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A68" t="s">
-        <v>496</v>
-      </c>
-      <c r="B68" t="s">
-        <v>497</v>
-      </c>
-      <c r="C68">
-        <v>2022</v>
-      </c>
-      <c r="D68">
-        <v>12</v>
-      </c>
-      <c r="E68" t="s">
-        <v>514</v>
-      </c>
-      <c r="F68" s="12" t="s">
-        <v>515</v>
-      </c>
-      <c r="G68" s="7" t="s">
-        <v>593</v>
-      </c>
-      <c r="H68" s="11">
-        <v>652905140123</v>
-      </c>
-      <c r="I68" t="s">
-        <v>663</v>
-      </c>
-      <c r="J68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A69" t="s">
-        <v>496</v>
-      </c>
-      <c r="B69" t="s">
-        <v>497</v>
-      </c>
-      <c r="C69">
-        <v>2022</v>
-      </c>
-      <c r="D69">
-        <v>12</v>
-      </c>
-      <c r="E69" t="s">
-        <v>514</v>
-      </c>
-      <c r="F69" s="12" t="s">
-        <v>515</v>
-      </c>
-      <c r="G69" s="7" t="s">
-        <v>594</v>
-      </c>
-      <c r="H69" s="11">
-        <v>652905140222</v>
-      </c>
-      <c r="I69" t="s">
-        <v>664</v>
-      </c>
-      <c r="J69">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A70" t="s">
-        <v>496</v>
-      </c>
-      <c r="B70" t="s">
-        <v>497</v>
-      </c>
-      <c r="C70">
-        <v>2022</v>
-      </c>
-      <c r="D70">
-        <v>12</v>
-      </c>
-      <c r="E70" t="s">
-        <v>514</v>
-      </c>
-      <c r="F70" s="12" t="s">
-        <v>515</v>
-      </c>
-      <c r="G70" s="7" t="s">
-        <v>595</v>
-      </c>
-      <c r="H70" s="9">
-        <v>652905140420</v>
-      </c>
-      <c r="I70" t="s">
-        <v>665</v>
-      </c>
-      <c r="J70">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A71" t="s">
-        <v>496</v>
-      </c>
-      <c r="B71" t="s">
-        <v>497</v>
-      </c>
-      <c r="C71">
-        <v>2022</v>
-      </c>
-      <c r="D71">
-        <v>12</v>
-      </c>
-      <c r="E71" t="s">
-        <v>514</v>
-      </c>
-      <c r="F71" s="12" t="s">
-        <v>515</v>
-      </c>
-      <c r="G71" s="7" t="s">
-        <v>596</v>
-      </c>
-      <c r="H71" s="9">
-        <v>652905140628</v>
-      </c>
-      <c r="I71" t="s">
-        <v>666</v>
-      </c>
-      <c r="J71">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A72" t="s">
-        <v>496</v>
-      </c>
-      <c r="B72" t="s">
-        <v>497</v>
-      </c>
-      <c r="C72">
-        <v>2022</v>
-      </c>
-      <c r="D72">
-        <v>12</v>
-      </c>
-      <c r="E72" t="s">
-        <v>514</v>
-      </c>
-      <c r="F72" s="10" t="s">
-        <v>520</v>
-      </c>
-      <c r="G72" s="7" t="s">
-        <v>597</v>
-      </c>
-      <c r="H72" s="9">
-        <v>652905150122</v>
-      </c>
-      <c r="I72" t="s">
-        <v>667</v>
-      </c>
-      <c r="J72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A73" t="s">
-        <v>496</v>
-      </c>
-      <c r="B73" t="s">
-        <v>497</v>
-      </c>
-      <c r="C73">
-        <v>2022</v>
-      </c>
-      <c r="D73">
-        <v>12</v>
-      </c>
-      <c r="E73" t="s">
-        <v>514</v>
-      </c>
-      <c r="F73" s="10" t="s">
-        <v>521</v>
-      </c>
-      <c r="G73" s="7" t="s">
-        <v>598</v>
-      </c>
-      <c r="H73" s="9">
-        <v>652905160121</v>
-      </c>
-      <c r="I73" t="s">
+      <c r="E77" s="9" t="s">
+        <v>523</v>
+      </c>
+      <c r="F77" s="12" t="s">
+        <v>599</v>
+      </c>
+      <c r="G77" s="8">
+        <v>652905180129</v>
+      </c>
+      <c r="H77" t="s">
         <v>668</v>
       </c>
-      <c r="J73">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A74" t="s">
-        <v>496</v>
-      </c>
-      <c r="B74" t="s">
-        <v>497</v>
-      </c>
-      <c r="C74">
-        <v>2022</v>
-      </c>
-      <c r="D74">
-        <v>12</v>
-      </c>
-      <c r="E74" t="s">
-        <v>516</v>
-      </c>
-      <c r="F74" s="10" t="s">
-        <v>521</v>
-      </c>
-      <c r="G74" s="7" t="s">
-        <v>599</v>
-      </c>
-      <c r="H74" s="9">
-        <v>652905160213</v>
-      </c>
-      <c r="I74" t="s">
-        <v>669</v>
-      </c>
-      <c r="J74">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A75" t="s">
-        <v>496</v>
-      </c>
-      <c r="B75" t="s">
-        <v>497</v>
-      </c>
-      <c r="C75">
-        <v>2022</v>
-      </c>
-      <c r="D75">
-        <v>12</v>
-      </c>
-      <c r="E75" t="s">
-        <v>514</v>
-      </c>
-      <c r="F75" s="10" t="s">
-        <v>521</v>
-      </c>
-      <c r="G75" s="7" t="s">
-        <v>600</v>
-      </c>
-      <c r="H75" s="9">
-        <v>652905160220</v>
-      </c>
-      <c r="I75" t="s">
-        <v>669</v>
-      </c>
-      <c r="J75">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A76" t="s">
-        <v>496</v>
-      </c>
-      <c r="B76" t="s">
-        <v>497</v>
-      </c>
-      <c r="C76">
-        <v>2022</v>
-      </c>
-      <c r="D76">
-        <v>12</v>
-      </c>
-      <c r="E76" t="s">
-        <v>514</v>
-      </c>
-      <c r="F76" s="10" t="s">
-        <v>523</v>
-      </c>
-      <c r="G76" s="7" t="s">
-        <v>601</v>
-      </c>
-      <c r="H76" s="9">
-        <v>652905170120</v>
-      </c>
-      <c r="I76" t="s">
-        <v>670</v>
-      </c>
-      <c r="J76">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A77" t="s">
-        <v>496</v>
-      </c>
-      <c r="B77" t="s">
-        <v>497</v>
-      </c>
-      <c r="C77">
-        <v>2022</v>
-      </c>
-      <c r="D77">
-        <v>12</v>
-      </c>
-      <c r="E77" t="s">
-        <v>514</v>
-      </c>
-      <c r="F77" s="10" t="s">
-        <v>526</v>
-      </c>
-      <c r="G77" s="7" t="s">
-        <v>602</v>
-      </c>
-      <c r="H77" s="9">
-        <v>652905180129</v>
-      </c>
-      <c r="I77" t="s">
-        <v>671</v>
-      </c>
-      <c r="J77" s="4">
+      <c r="I77" s="4">
         <v>258</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F39 F2:F18">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E39 E2:E18">
       <formula1>100</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>